<commit_message>
hotfix event Squashed commit of the following:
commit f8724b9ffd157c63e123fb44f3edd097203506d2
Author: Vick Scarlet <scarlet_vick@outlook.com>
Date:   Sat Jan 29 01:08:39 2022 +0800

    update event
</commit_message>
<xml_diff>
--- a/data/en-us/achievement.xlsx
+++ b/data/en-us/achievement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\84694\Desktop\人生重来\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192AAC15-664F-426D-8674-7964E8F2D586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209A061E-CC5D-4A1F-83F8-6A8356193134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="achievement" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="513">
   <si>
     <t>$id</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -2052,10 +2052,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>(ATLT?[1023])&amp;(ATLT?[1048])&amp;(ATLT?[1064])&amp;(ATLT?[1114])&amp;(ATLT?[1135])&amp;(ATLT?[1141])</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>有会员，所以急着投胎</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -2077,6 +2073,46 @@
   </si>
   <si>
     <t>太贪婪而被骗</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TLT?[2036]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>自 投 罗 网</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>经 典 老 歌</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>集齐四大悲剧</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>莎比</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(ATLT?[2028])&amp;(ATLT?[2029])&amp;(ATLT?[2030])&amp;(ATLT?[2031])</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>死了但没完全死</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>死而复生</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>EVT?[20000,20001,11504]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>(ATLT?[1023])&amp;(ATLT?[1048])&amp;(ATLT?[1064])&amp;(ATLT?[1114])&amp;(ATLT?[1135])&amp;(ATLT?[1141])&amp;(ATLT?[1147])</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2464,28 +2500,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M166"/>
+  <dimension ref="A1:M168"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A159" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C165" sqref="C165"/>
+      <pane ySplit="2" topLeftCell="A150" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G122" sqref="G122"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="25.44140625" defaultRowHeight="19.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="25.5" defaultRowHeight="20.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.44140625" style="5"/>
-    <col min="2" max="2" width="27.44140625" style="5" customWidth="1"/>
+    <col min="1" max="1" width="25.5" style="5"/>
+    <col min="2" max="2" width="27.5" style="5" customWidth="1"/>
     <col min="3" max="3" width="33" style="5" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="11.125" style="5" customWidth="1"/>
     <col min="5" max="5" width="62" customWidth="1"/>
-    <col min="6" max="6" width="15.109375" style="5" customWidth="1"/>
-    <col min="7" max="7" width="56.77734375" style="5" customWidth="1"/>
-    <col min="8" max="10" width="13.5546875" style="5" customWidth="1"/>
-    <col min="11" max="13" width="18.88671875" style="6" customWidth="1"/>
-    <col min="14" max="16384" width="25.44140625" style="5"/>
+    <col min="6" max="6" width="15.125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="56.75" style="5" customWidth="1"/>
+    <col min="8" max="10" width="13.5" style="5" customWidth="1"/>
+    <col min="11" max="13" width="18.875" style="6" customWidth="1"/>
+    <col min="14" max="16384" width="25.5" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2511,7 +2547,7 @@
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
     </row>
-    <row r="2" spans="1:13" s="3" customFormat="1" ht="109.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="3" customFormat="1" ht="109.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -2538,7 +2574,7 @@
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
     </row>
-    <row r="3" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5">
         <v>101</v>
       </c>
@@ -2561,7 +2597,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5">
         <v>102</v>
       </c>
@@ -2584,7 +2620,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
         <v>103</v>
       </c>
@@ -2607,7 +2643,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5">
         <v>104</v>
       </c>
@@ -2630,7 +2666,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5">
         <v>105</v>
       </c>
@@ -2653,7 +2689,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
         <v>106</v>
       </c>
@@ -2676,7 +2712,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>107</v>
       </c>
@@ -2699,7 +2735,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="5">
         <v>108</v>
       </c>
@@ -2722,7 +2758,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>109</v>
       </c>
@@ -2745,7 +2781,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>110</v>
       </c>
@@ -2768,7 +2804,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
         <v>111</v>
       </c>
@@ -2791,7 +2827,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
         <v>112</v>
       </c>
@@ -2814,7 +2850,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5">
         <v>113</v>
       </c>
@@ -2837,7 +2873,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5">
         <v>114</v>
       </c>
@@ -2860,7 +2896,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5">
         <v>115</v>
       </c>
@@ -2883,7 +2919,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5">
         <v>116</v>
       </c>
@@ -2906,7 +2942,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5">
         <v>117</v>
       </c>
@@ -2929,7 +2965,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5">
         <v>118</v>
       </c>
@@ -2952,7 +2988,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5">
         <v>119</v>
       </c>
@@ -2975,7 +3011,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5">
         <v>120</v>
       </c>
@@ -2998,7 +3034,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5">
         <v>121</v>
       </c>
@@ -3021,7 +3057,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5">
         <v>122</v>
       </c>
@@ -3044,7 +3080,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="5">
         <v>123</v>
       </c>
@@ -3067,7 +3103,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="5">
         <v>124</v>
       </c>
@@ -3090,7 +3126,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="5">
         <v>125</v>
       </c>
@@ -3113,7 +3149,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="5">
         <v>126</v>
       </c>
@@ -3136,7 +3172,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="5">
         <v>127</v>
       </c>
@@ -3159,7 +3195,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="5">
         <v>128</v>
       </c>
@@ -3182,7 +3218,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="5">
         <v>129</v>
       </c>
@@ -3205,7 +3241,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="5">
         <v>130</v>
       </c>
@@ -3228,7 +3264,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5">
         <v>131</v>
       </c>
@@ -3251,7 +3287,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="5">
         <v>132</v>
       </c>
@@ -3274,7 +3310,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="5">
         <v>133</v>
       </c>
@@ -3297,7 +3333,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="5">
         <v>134</v>
       </c>
@@ -3320,7 +3356,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="5">
         <v>135</v>
       </c>
@@ -3343,7 +3379,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="5">
         <v>136</v>
       </c>
@@ -3366,7 +3402,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="5">
         <v>137</v>
       </c>
@@ -3389,7 +3425,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="5">
         <v>138</v>
       </c>
@@ -3412,7 +3448,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="5">
         <v>139</v>
       </c>
@@ -3435,7 +3471,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="5">
         <v>140</v>
       </c>
@@ -3458,7 +3494,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="5">
         <v>141</v>
       </c>
@@ -3481,7 +3517,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="5">
         <v>142</v>
       </c>
@@ -3504,7 +3540,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="5">
         <v>143</v>
       </c>
@@ -3527,7 +3563,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="5">
         <v>144</v>
       </c>
@@ -3550,7 +3586,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="5">
         <v>145</v>
       </c>
@@ -3573,7 +3609,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="5">
         <v>146</v>
       </c>
@@ -3596,7 +3632,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="5">
         <v>147</v>
       </c>
@@ -3619,7 +3655,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="5">
         <v>148</v>
       </c>
@@ -3642,7 +3678,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="5">
         <v>149</v>
       </c>
@@ -3665,7 +3701,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="5">
         <v>150</v>
       </c>
@@ -3688,7 +3724,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="5">
         <v>151</v>
       </c>
@@ -3711,7 +3747,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="5">
         <v>152</v>
       </c>
@@ -3734,7 +3770,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="5">
         <v>153</v>
       </c>
@@ -3757,7 +3793,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="5">
         <v>154</v>
       </c>
@@ -3780,7 +3816,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="5">
         <v>155</v>
       </c>
@@ -3803,7 +3839,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="5">
         <v>156</v>
       </c>
@@ -3826,7 +3862,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="5">
         <v>157</v>
       </c>
@@ -3849,7 +3885,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="5">
         <v>158</v>
       </c>
@@ -3872,7 +3908,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="5">
         <v>159</v>
       </c>
@@ -3895,7 +3931,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="5">
         <v>160</v>
       </c>
@@ -3918,7 +3954,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="5">
         <v>161</v>
       </c>
@@ -3941,7 +3977,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="5">
         <v>162</v>
       </c>
@@ -3964,7 +4000,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="5">
         <v>163</v>
       </c>
@@ -3987,7 +4023,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="5">
         <v>164</v>
       </c>
@@ -4010,7 +4046,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="5">
         <v>165</v>
       </c>
@@ -4033,7 +4069,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="5">
         <v>166</v>
       </c>
@@ -4056,7 +4092,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="5">
         <v>167</v>
       </c>
@@ -4079,7 +4115,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="5">
         <v>168</v>
       </c>
@@ -4102,7 +4138,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="5">
         <v>169</v>
       </c>
@@ -4125,7 +4161,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="5">
         <v>170</v>
       </c>
@@ -4148,7 +4184,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="5">
         <v>171</v>
       </c>
@@ -4171,7 +4207,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="5">
         <v>172</v>
       </c>
@@ -4194,7 +4230,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="5">
         <v>173</v>
       </c>
@@ -4217,7 +4253,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="5">
         <v>174</v>
       </c>
@@ -4240,7 +4276,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="5">
         <v>175</v>
       </c>
@@ -4263,7 +4299,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="5">
         <v>176</v>
       </c>
@@ -4286,7 +4322,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="5">
         <v>177</v>
       </c>
@@ -4309,7 +4345,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="5">
         <v>178</v>
       </c>
@@ -4332,7 +4368,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="5">
         <v>179</v>
       </c>
@@ -4355,7 +4391,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="5">
         <v>180</v>
       </c>
@@ -4378,7 +4414,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="5">
         <v>181</v>
       </c>
@@ -4401,7 +4437,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="5">
         <v>182</v>
       </c>
@@ -4424,7 +4460,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="5">
         <v>183</v>
       </c>
@@ -4447,7 +4483,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="5">
         <v>184</v>
       </c>
@@ -4470,7 +4506,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="5">
         <v>185</v>
       </c>
@@ -4493,7 +4529,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="5">
         <v>186</v>
       </c>
@@ -4516,7 +4552,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="5">
         <v>187</v>
       </c>
@@ -4539,7 +4575,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="5">
         <v>188</v>
       </c>
@@ -4562,7 +4598,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="5">
         <v>189</v>
       </c>
@@ -4585,7 +4621,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="5">
         <v>190</v>
       </c>
@@ -4608,7 +4644,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="5">
         <v>191</v>
       </c>
@@ -4631,7 +4667,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="5">
         <v>192</v>
       </c>
@@ -4654,7 +4690,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="5">
         <v>193</v>
       </c>
@@ -4677,7 +4713,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="5">
         <v>194</v>
       </c>
@@ -4700,7 +4736,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="5">
         <v>195</v>
       </c>
@@ -4723,7 +4759,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="5">
         <v>196</v>
       </c>
@@ -4746,7 +4782,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="5">
         <v>197</v>
       </c>
@@ -4769,7 +4805,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="5">
         <v>198</v>
       </c>
@@ -4792,7 +4828,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="5">
         <v>199</v>
       </c>
@@ -4815,7 +4851,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="5">
         <v>200</v>
       </c>
@@ -4838,7 +4874,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="5">
         <v>201</v>
       </c>
@@ -4861,7 +4897,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="5">
         <v>202</v>
       </c>
@@ -4884,7 +4920,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="5">
         <v>203</v>
       </c>
@@ -4907,7 +4943,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="5">
         <v>204</v>
       </c>
@@ -4930,7 +4966,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="5">
         <v>205</v>
       </c>
@@ -4953,7 +4989,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="5">
         <v>206</v>
       </c>
@@ -4976,7 +5012,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="5">
         <v>207</v>
       </c>
@@ -4999,7 +5035,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="5">
         <v>208</v>
       </c>
@@ -5022,7 +5058,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="5">
         <v>209</v>
       </c>
@@ -5045,7 +5081,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="5">
         <v>210</v>
       </c>
@@ -5068,7 +5104,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="5">
         <v>211</v>
       </c>
@@ -5091,7 +5127,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="5">
         <v>212</v>
       </c>
@@ -5114,7 +5150,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="5">
         <v>213</v>
       </c>
@@ -5137,7 +5173,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="5">
         <v>214</v>
       </c>
@@ -5160,7 +5196,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="5">
         <v>215</v>
       </c>
@@ -5183,7 +5219,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="5">
         <v>216</v>
       </c>
@@ -5206,7 +5242,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="5">
         <v>217</v>
       </c>
@@ -5229,7 +5265,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="5">
         <v>218</v>
       </c>
@@ -5252,7 +5288,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="5">
         <v>219</v>
       </c>
@@ -5266,7 +5302,7 @@
         <v>3</v>
       </c>
       <c r="E121" s="5" t="s">
-        <v>497</v>
+        <v>512</v>
       </c>
       <c r="F121" s="5">
         <v>0</v>
@@ -5275,7 +5311,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="5">
         <v>220</v>
       </c>
@@ -5298,7 +5334,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="5">
         <v>221</v>
       </c>
@@ -5321,7 +5357,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="5">
         <v>222</v>
       </c>
@@ -5344,7 +5380,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="5">
         <v>223</v>
       </c>
@@ -5367,7 +5403,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="5">
         <v>224</v>
       </c>
@@ -5390,7 +5426,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="5">
         <v>225</v>
       </c>
@@ -5413,7 +5449,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="5">
         <v>226</v>
       </c>
@@ -5436,7 +5472,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="5">
         <v>227</v>
       </c>
@@ -5459,7 +5495,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="5">
         <v>228</v>
       </c>
@@ -5482,7 +5518,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="5">
         <v>229</v>
       </c>
@@ -5505,7 +5541,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="5">
         <v>230</v>
       </c>
@@ -5528,7 +5564,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="5">
         <v>231</v>
       </c>
@@ -5551,7 +5587,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="5">
         <v>232</v>
       </c>
@@ -5574,7 +5610,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="135" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="5">
         <v>233</v>
       </c>
@@ -5597,7 +5633,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="136" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="5">
         <v>234</v>
       </c>
@@ -5620,7 +5656,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="5">
         <v>235</v>
       </c>
@@ -5643,7 +5679,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="5">
         <v>236</v>
       </c>
@@ -5666,7 +5702,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="139" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="5">
         <v>237</v>
       </c>
@@ -5689,7 +5725,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="5">
         <v>238</v>
       </c>
@@ -5712,7 +5748,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="141" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="5">
         <v>239</v>
       </c>
@@ -5735,7 +5771,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="142" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="5">
         <v>240</v>
       </c>
@@ -5758,7 +5794,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="143" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="5">
         <v>241</v>
       </c>
@@ -5781,7 +5817,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="144" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="5">
         <v>242</v>
       </c>
@@ -5804,7 +5840,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="145" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="5">
         <v>243</v>
       </c>
@@ -5827,7 +5863,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="146" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="5">
         <v>244</v>
       </c>
@@ -5850,7 +5886,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="147" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="5">
         <v>245</v>
       </c>
@@ -5873,7 +5909,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="148" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="5">
         <v>246</v>
       </c>
@@ -5896,7 +5932,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="149" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="5">
         <v>247</v>
       </c>
@@ -5919,7 +5955,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="150" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="5">
         <v>248</v>
       </c>
@@ -5942,7 +5978,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="151" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="5">
         <v>249</v>
       </c>
@@ -5965,7 +6001,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="152" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="5">
         <v>250</v>
       </c>
@@ -5988,7 +6024,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="153" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="5">
         <v>251</v>
       </c>
@@ -6011,7 +6047,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="154" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="5">
         <v>252</v>
       </c>
@@ -6034,7 +6070,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="155" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="5">
         <v>253</v>
       </c>
@@ -6057,7 +6093,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="156" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="5">
         <v>254</v>
       </c>
@@ -6080,7 +6116,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="157" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="5">
         <v>255</v>
       </c>
@@ -6103,7 +6139,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="158" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="5">
         <v>256</v>
       </c>
@@ -6126,7 +6162,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="159" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="5">
         <v>257</v>
       </c>
@@ -6149,7 +6185,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="160" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="5">
         <v>258</v>
       </c>
@@ -6172,7 +6208,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="161" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="5">
         <v>259</v>
       </c>
@@ -6195,7 +6231,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="162" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="5">
         <v>260</v>
       </c>
@@ -6218,21 +6254,21 @@
         <v>440</v>
       </c>
     </row>
-    <row r="163" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="5">
         <v>261</v>
       </c>
       <c r="B163" s="5" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C163" s="5" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D163" s="5">
         <v>2</v>
       </c>
       <c r="E163" s="5" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F163" s="5">
         <v>0</v>
@@ -6241,21 +6277,21 @@
         <v>441</v>
       </c>
     </row>
-    <row r="164" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="5">
         <v>262</v>
       </c>
       <c r="B164" s="5" t="s">
+        <v>500</v>
+      </c>
+      <c r="C164" s="5" t="s">
+        <v>502</v>
+      </c>
+      <c r="D164" s="5">
+        <v>0</v>
+      </c>
+      <c r="E164" s="5" t="s">
         <v>501</v>
-      </c>
-      <c r="C164" s="5" t="s">
-        <v>503</v>
-      </c>
-      <c r="D164" s="5">
-        <v>0</v>
-      </c>
-      <c r="E164" s="5" t="s">
-        <v>502</v>
       </c>
       <c r="F164" s="5">
         <v>1</v>
@@ -6264,11 +6300,77 @@
         <v>441</v>
       </c>
     </row>
-    <row r="165" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E165" s="5"/>
-    </row>
-    <row r="166" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E166" s="5"/>
+    <row r="165" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A165" s="5">
+        <v>263</v>
+      </c>
+      <c r="B165" s="5" t="s">
+        <v>505</v>
+      </c>
+      <c r="C165" s="5" t="s">
+        <v>504</v>
+      </c>
+      <c r="D165" s="5">
+        <v>2</v>
+      </c>
+      <c r="E165" s="5" t="s">
+        <v>503</v>
+      </c>
+      <c r="F165" s="5">
+        <v>1</v>
+      </c>
+      <c r="G165" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A166" s="5">
+        <v>264</v>
+      </c>
+      <c r="B166" s="5" t="s">
+        <v>507</v>
+      </c>
+      <c r="C166" s="5" t="s">
+        <v>506</v>
+      </c>
+      <c r="D166" s="5">
+        <v>2</v>
+      </c>
+      <c r="E166" s="5" t="s">
+        <v>508</v>
+      </c>
+      <c r="F166" s="5">
+        <v>0</v>
+      </c>
+      <c r="G166" s="5" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A167" s="5">
+        <v>265</v>
+      </c>
+      <c r="B167" s="5" t="s">
+        <v>509</v>
+      </c>
+      <c r="C167" s="5" t="s">
+        <v>510</v>
+      </c>
+      <c r="D167" s="5">
+        <v>2</v>
+      </c>
+      <c r="E167" s="5" t="s">
+        <v>511</v>
+      </c>
+      <c r="F167" s="5">
+        <v>0</v>
+      </c>
+      <c r="G167" s="5" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E168" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>